<commit_message>
Updates to files and structure
More additions to proposal and asset list spreadsheet. added audio folder with a README for what it will contain
</commit_message>
<xml_diff>
--- a/documentation/Sound Asset List.xlsx
+++ b/documentation/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30057398-9ADF-4033-81FD-AF41D7A07B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E358C44-42BD-467F-85AD-ACED242C2B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Dialog</t>
   </si>
@@ -55,6 +55,105 @@
   </si>
   <si>
     <t>Voiceover (robotized)</t>
+  </si>
+  <si>
+    <t>Initial game startup</t>
+  </si>
+  <si>
+    <t>Ambience</t>
+  </si>
+  <si>
+    <t>Hollow, drawn out noises like you would hear in space movies</t>
+  </si>
+  <si>
+    <t>Player is in-game (constant background ambience)</t>
+  </si>
+  <si>
+    <t>More hollow, echoing space sounds</t>
+  </si>
+  <si>
+    <t>Space traversal music, general game background noises/ambience</t>
+  </si>
+  <si>
+    <t>Player changes the tilt position of the ship (Q/E)</t>
+  </si>
+  <si>
+    <t>Ship rotates side to side, release a ping adjustment sound</t>
+  </si>
+  <si>
+    <t>Sound Effect</t>
+  </si>
+  <si>
+    <t>A pinging sound. Like a submarine but with less echo</t>
+  </si>
+  <si>
+    <t>Main menu theme (think Mass Effect but less music/less serious)</t>
+  </si>
+  <si>
+    <t>Player moves ship forwards</t>
+  </si>
+  <si>
+    <t>Player moves ship backwards</t>
+  </si>
+  <si>
+    <t>Ship moves forwards, deep whooshing noise that gets higher in tone as time goes on</t>
+  </si>
+  <si>
+    <t>Whoosh effect, higher tones as it continues</t>
+  </si>
+  <si>
+    <t>Whoosh effect, deeper tones as it continues</t>
+  </si>
+  <si>
+    <t>Ship moves backwards, deep whoosing noise that gets lower in tone as time goes on</t>
+  </si>
+  <si>
+    <t>Player turns ship left or right</t>
+  </si>
+  <si>
+    <t>Ship turns to either side, lower whooshing tone so as not to interfere with forward or backward sounds</t>
+  </si>
+  <si>
+    <t>Player presses enter to begin game</t>
+  </si>
+  <si>
+    <t>Echoing ding-like sound; indicates that the player pressed a key to start</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Player hits escape to enter the pause menu</t>
+  </si>
+  <si>
+    <t>Player approaches one of the astronauts</t>
+  </si>
+  <si>
+    <t>Sound Effect/Dialog</t>
+  </si>
+  <si>
+    <t>Astronaut sends an SOS signal over their radio, gets louder as ship approaches</t>
+  </si>
+  <si>
+    <t>High-tech sound, like a TV screen turning on; electric sound, "futuristic user interface" sound</t>
+  </si>
+  <si>
+    <t>Another whoosh, lower register</t>
+  </si>
+  <si>
+    <t>high-pitched whir, electric buzz</t>
+  </si>
+  <si>
+    <t>A solid dinging noise</t>
+  </si>
+  <si>
+    <t>distress signal, voiceover</t>
+  </si>
+  <si>
+    <t>Player picks up an astronaut (runs into them with the ship)</t>
+  </si>
+  <si>
+    <t>*Sound List subject to additions or changes*</t>
   </si>
 </sst>
 </file>
@@ -100,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,16 +207,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0">
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -401,16 +515,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70.28515625" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
@@ -433,24 +547,188 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Asset List and Almost Finished Proposal
Asset list for sounds is done (for now). Proposal will be done later. 3 sound design explanations left.
</commit_message>
<xml_diff>
--- a/documentation/Sound Asset List.xlsx
+++ b/documentation/Sound Asset List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E358C44-42BD-467F-85AD-ACED242C2B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E03EC5-2431-4839-9ED0-303E80B2E799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Dialog</t>
   </si>
@@ -154,6 +154,63 @@
   </si>
   <si>
     <t>*Sound List subject to additions or changes*</t>
+  </si>
+  <si>
+    <t>Ship picks up the astronaut, multiple rapid pinging sounds to indicate success</t>
+  </si>
+  <si>
+    <t>Effect Name</t>
+  </si>
+  <si>
+    <t>MainMenuTheme</t>
+  </si>
+  <si>
+    <t>dinging sound, metal windchime noise</t>
+  </si>
+  <si>
+    <t>StartGame</t>
+  </si>
+  <si>
+    <t>DialogIntro</t>
+  </si>
+  <si>
+    <t>SpaceAmbience</t>
+  </si>
+  <si>
+    <t>ShipTilt</t>
+  </si>
+  <si>
+    <t>ShipForward</t>
+  </si>
+  <si>
+    <t>ShipBackward</t>
+  </si>
+  <si>
+    <t>ShipSideways</t>
+  </si>
+  <si>
+    <t>EnterPauseMenu</t>
+  </si>
+  <si>
+    <t>AstronautDistressCall</t>
+  </si>
+  <si>
+    <t>CollectAstronaut</t>
+  </si>
+  <si>
+    <t>PauseMenuAmbience</t>
+  </si>
+  <si>
+    <t>Player enters pause menu</t>
+  </si>
+  <si>
+    <t>Pause menu theme (likely a "remix" of the main menu theme)</t>
+  </si>
+  <si>
+    <t>Ambience/Music</t>
+  </si>
+  <si>
+    <t>More space movie sounds, hollow, slightly different from main menu sounds</t>
   </si>
 </sst>
 </file>
@@ -515,215 +572,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>